<commit_message>
updates for the path detection simulation.
</commit_message>
<xml_diff>
--- a/sandbox/NHANES/input/Dictionary_1516.xlsx
+++ b/sandbox/NHANES/input/Dictionary_1516.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidmccoy/SuperNOVA/sandbox/NHANES/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18995568-C775-0448-AB12-1B9B25CA8A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF54A4-36F5-A045-8B5F-130BE4244074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1840" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{F5BC8812-2267-1A4E-A624-4E8111A7A57C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{F5BC8812-2267-1A4E-A624-4E8111A7A57C}"/>
   </bookViews>
   <sheets>
     <sheet name="total" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11019" uniqueCount="7664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11039" uniqueCount="7683">
   <si>
     <t>Variable Name</t>
   </si>
@@ -23019,13 +23019,70 @@
   </si>
   <si>
     <t>Asthma</t>
+  </si>
+  <si>
+    <t>C_Reactive_Protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha_carotene </t>
+  </si>
+  <si>
+    <t>LBXBEC</t>
+  </si>
+  <si>
+    <t>beta_carotene</t>
+  </si>
+  <si>
+    <t>LBXVIA</t>
+  </si>
+  <si>
+    <t>vitamin_a</t>
+  </si>
+  <si>
+    <t>LBXVIE</t>
+  </si>
+  <si>
+    <t>vitamin_e</t>
+  </si>
+  <si>
+    <t>LBXLYC</t>
+  </si>
+  <si>
+    <t>trans_lycopene</t>
+  </si>
+  <si>
+    <t>LBDTLY</t>
+  </si>
+  <si>
+    <t>total_lycopene</t>
+  </si>
+  <si>
+    <t>LBXLUZ</t>
+  </si>
+  <si>
+    <t>LBXCRY</t>
+  </si>
+  <si>
+    <t>b_Cryptoxanthin</t>
+  </si>
+  <si>
+    <t>LBXGTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g_Tocopherol </t>
+  </si>
+  <si>
+    <t>lutein_and_zeaxanthin</t>
+  </si>
+  <si>
+    <t>LBXALC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23092,6 +23149,12 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF374151"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -23120,7 +23183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -23132,6 +23195,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23449,7 +23513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E09E9E5-8805-2548-B7DD-F640EF627B88}">
   <dimension ref="A1:B5376"/>
   <sheetViews>
-    <sheetView topLeftCell="A3274" workbookViewId="0">
+    <sheetView topLeftCell="A5363" workbookViewId="0">
       <selection activeCell="B2885" sqref="B2885"/>
     </sheetView>
   </sheetViews>
@@ -66444,10 +66508,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71155A1-5685-B745-B778-438C55847435}">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -67550,6 +67614,86 @@
       </c>
       <c r="B137" s="10" t="s">
         <v>7663</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
+        <v>7625</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>7664</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
+        <v>7682</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>7665</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="A140" s="7" t="s">
+        <v>7666</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>7667</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="A141" s="11" t="s">
+        <v>7668</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>7669</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="A142" s="11" t="s">
+        <v>7670</v>
+      </c>
+      <c r="B142" s="10" t="s">
+        <v>7671</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A143" s="11" t="s">
+        <v>7672</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>7673</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A144" s="11" t="s">
+        <v>7674</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>7675</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A145" s="11" t="s">
+        <v>7676</v>
+      </c>
+      <c r="B145" s="11" t="s">
+        <v>7681</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A146" s="11" t="s">
+        <v>7677</v>
+      </c>
+      <c r="B146" s="11" t="s">
+        <v>7678</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A147" s="11" t="s">
+        <v>7679</v>
+      </c>
+      <c r="B147" s="11" t="s">
+        <v>7680</v>
       </c>
     </row>
   </sheetData>
@@ -67600,6 +67744,9 @@
     <hyperlink ref="B118" r:id="rId44" location="URXUPT" display="https://wwwn.cdc.gov/Nchs/Nhanes/2001-2002/L06HM_B.htm - URXUPT" xr:uid="{5820B416-49D9-C24E-B155-B057B2319A0B}"/>
     <hyperlink ref="A130" r:id="rId45" location="PAQ180" display="https://wwwn.cdc.gov/nchs/nhanes/1999-2000/PAQ.htm - PAQ180" xr:uid="{9B3DBC61-7381-5944-8159-FF3906036F4B}"/>
     <hyperlink ref="B130" r:id="rId46" location="PAQ180" display="https://wwwn.cdc.gov/nchs/nhanes/1999-2000/PAQ.htm - PAQ180" xr:uid="{9F0C8902-04EC-DD4E-8131-5D23F6F90DF2}"/>
+    <hyperlink ref="A138" r:id="rId47" location="LBXCRP" display="https://wwwn.cdc.gov/nchs/nhanes/2003-2004/L11_C.htm - LBXCRP" xr:uid="{83EFCFDA-858D-1D44-ADF5-485B1F1BD0C2}"/>
+    <hyperlink ref="A139" r:id="rId48" location="LBXALC" display="https://wwwn.cdc.gov/nchs/nhanes/2005-2006/VITAEC_D.htm - LBXALC" xr:uid="{E9F3A6CB-D1A3-D240-BBEA-527F02C2BEEB}"/>
+    <hyperlink ref="A140" r:id="rId49" location="LBXBEC" display="https://wwwn.cdc.gov/nchs/nhanes/2005-2006/VITAEC_D.htm - LBXBEC" xr:uid="{705181B4-6F5B-E645-A85D-A7C2EBAB3854}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>